<commit_message>
Implemented IBusinessObjectRule that can be added to the BusinessObject.BusinessObjectRules and is validated with Status.IsValid and Status.HasWarnings Removed or fixed many todo's Removed Classes such as PropRuleObject that are not being used.
</commit_message>
<xml_diff>
--- a/docs/PriorityList.xlsx
+++ b/docs/PriorityList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="20895" windowHeight="12210"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>Started W/out peter</t>
   </si>
@@ -54,6 +54,127 @@
   </si>
   <si>
     <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Model Business Objects. I.e. Build easy to use – user interfaces using Habanero Business Objects. Use a normal database to start.</t>
+    </r>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <r>
+      <t>c.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Track what has been generated and what has been changed s.t. can control generation i.e. if the class has been generated then don’t regenerate also need to be able to do this for relationships or properties. I.e. if you override the relationship behaviour then want to be able to not regenerate.</t>
+    </r>
+  </si>
+  <si>
+    <t>9 dep b</t>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Reorganise Habanero.Base</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Check For Duplicates in same transaction as commit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Generate Forms</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>a.</t>
     </r>
     <r>
@@ -72,7 +193,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Reverse Engineering from Database. Pluggable such that can extend to any database easily. Need to be able</t>
+      <t>Simple CRUD Grid - Read only Grid, Editable Grid</t>
     </r>
   </si>
   <si>
@@ -95,11 +216,8 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Model Business Objects. I.e. Build easy to use – user interfaces using Habanero Business Objects. Use a normal database to start.</t>
-    </r>
-  </si>
-  <si>
-    <t>Y</t>
+      <t>CRUD Editor Form – Selector and BO Editor.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -121,7 +239,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Track what has been generated and what has been changed s.t. can control generation i.e. if the class has been generated then don’t regenerate also need to be able to do this for relationships or properties. I.e. if you override the relationship behaviour then want to be able to not regenerate.</t>
+      <t>Parent Child Form (Master – Child). Select master (possibly edit) get list of children select child edit. E.g. Customer – Orders.</t>
     </r>
   </si>
   <si>
@@ -144,12 +262,35 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Generate to code. Must be written such that can plug other templates into generator.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>e.</t>
+      <t>Generate tests</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>FindBy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
     </r>
     <r>
       <rPr>
@@ -167,15 +308,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Save the Business Model to XML instead of a database</t>
-    </r>
-  </si>
-  <si>
-    <t>9 dep b</t>
-  </si>
-  <si>
-    <r>
-      <t>2.</t>
+      <t>Create classes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
     </r>
     <r>
       <rPr>
@@ -193,127 +331,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Reorganise Habanero.Base</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Check For Duplicates in same transaction as commit</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>4.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Lookups Define philosophy and rework</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>5.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Relationships define philosophy and implement</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>6.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Generate Tests for BO’s</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>7.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Generate Forms</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a.</t>
+      <t>Generate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c.</t>
     </r>
     <r>
       <rPr>
@@ -331,104 +354,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Simple CRUD Grid - Read only Grid, Editable Grid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>CRUD Editor Form – Selector and BO Editor.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>c.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Parent Child Form (Master – Child). Select master (possibly edit) get list of children select child edit. E.g. Customer – Orders.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>d.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Generate tests</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>8.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Generate Database Structure and manage versions of application with different databases. (dep 1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.</t>
+      <t>Investigate LINQ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12.</t>
     </r>
     <r>
       <rPr>
@@ -446,81 +377,15 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>FindBy</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Create classes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>b.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Generate</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>c.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Investigate LINQ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>11.</t>
+      <t>Develop a set of UI test utils</t>
+    </r>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <r>
+      <t>13.</t>
     </r>
     <r>
       <rPr>
@@ -538,12 +403,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Gen/Dynamically define search criteria in ClassDefs for a Grid (dep 1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>12.</t>
+      <t>Study WPF, Silverlight etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>14.</t>
     </r>
     <r>
       <rPr>
@@ -561,15 +426,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Develop a set of UI test utils</t>
-    </r>
-  </si>
-  <si>
-    <t>ongoing</t>
-  </si>
-  <si>
-    <r>
-      <t>13.</t>
+      <t>Define Triggers in ClassDefs (dep on 9)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>16.</t>
     </r>
     <r>
       <rPr>
@@ -587,12 +449,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Study WPF, Silverlight etc</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>14.</t>
+      <t>Globalisation of all error messages.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>17.</t>
     </r>
     <r>
       <rPr>
@@ -610,12 +472,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Define Triggers in ClassDefs (dep on 9)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>15.</t>
+      <t>Email error messages</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>18.</t>
     </r>
     <r>
       <rPr>
@@ -633,12 +495,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Mutable Composite primary key for Readonly and editable grid. Sample app using Northwind.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>16.</t>
+      <t>Have option to do an SDI interface.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>19.</t>
     </r>
     <r>
       <rPr>
@@ -656,12 +518,15 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Globalisation of all error messages.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>17.</t>
+      <t>Allow multiple class defs for a project.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dep 25</t>
+  </si>
+  <si>
+    <r>
+      <t>22.</t>
     </r>
     <r>
       <rPr>
@@ -679,12 +544,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Email error messages</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>18.</t>
+      <t>Create Display objects i.e. object that can load based on any defined SQL load (allow summing, counting and other aggregate functions) and cannot be edited. This will replace loading these through a view.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>23.</t>
     </r>
     <r>
       <rPr>
@@ -702,12 +567,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Have option to do an SDI interface.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>19.</t>
+      <t>Allow the plugging in of any Database mapping logic for both reading and writing.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>24.</t>
     </r>
     <r>
       <rPr>
@@ -725,12 +590,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Allow multiple class defs for a project.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>20.</t>
+      <t>Create N-Tier Demo.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>25.</t>
     </r>
     <r>
       <rPr>
@@ -748,12 +613,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Allow bulk deleting of rows in a grid.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>21.</t>
+      <t>Serialisable Business objects and collections.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>26.</t>
     </r>
     <r>
       <rPr>
@@ -771,15 +636,15 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Create functionality to allow the object and collection to dump its state. See Serialisable</t>
-    </r>
-  </si>
-  <si>
-    <t>Dep 25</t>
-  </si>
-  <si>
-    <r>
-      <t>22.</t>
+      <t>Compact framework investigation</t>
+    </r>
+  </si>
+  <si>
+    <t>R&amp;D</t>
+  </si>
+  <si>
+    <r>
+      <t>27.</t>
     </r>
     <r>
       <rPr>
@@ -797,12 +662,15 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Create Display objects i.e. object that can load based on any defined SQL load (allow summing, counting and other aggregate functions) and cannot be edited. This will replace loading these through a view.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>23.</t>
+      <t>Reports (dep 22)</t>
+    </r>
+  </si>
+  <si>
+    <t>Dep 22</t>
+  </si>
+  <si>
+    <r>
+      <t>28.</t>
     </r>
     <r>
       <rPr>
@@ -820,154 +688,10 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Allow the plugging in of any Database mapping logic for both reading and writing.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>24.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Create N-Tier Demo.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>25.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Serialisable Business objects and collections.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>26.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Compact framework investigation</t>
-    </r>
-  </si>
-  <si>
-    <t>R&amp;D</t>
-  </si>
-  <si>
-    <r>
-      <t>27.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Reports (dep 22)</t>
-    </r>
-  </si>
-  <si>
-    <t>Dep 22</t>
-  </si>
-  <si>
-    <r>
-      <t>28.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>Support generation of VB.Net code.</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>29.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Collapsible Panel</t>
-    </r>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -978,6 +702,51 @@
   </si>
   <si>
     <t>9.      Refactor Panel Factory</t>
+  </si>
+  <si>
+    <t>a.       Reverse Engineering from Database. Pluggable such that can extend to any database easily. Need to be able</t>
+  </si>
+  <si>
+    <t>6.      Generate Tests for BO’s</t>
+  </si>
+  <si>
+    <t>d.      Generate to code. Must be written such that can plug other templates into generator.</t>
+  </si>
+  <si>
+    <t>Customisation - e.g. auto create guid id property etc</t>
+  </si>
+  <si>
+    <t>Eric and Donald</t>
+  </si>
+  <si>
+    <t>Mark Dee</t>
+  </si>
+  <si>
+    <t>11.  Gen/Dynamically define search criteria in ClassDefs for a Grid (dep 1)</t>
+  </si>
+  <si>
+    <t>15.  Mutable Composite primary key for Readonly and editable grid. Sample app using Northwind.</t>
+  </si>
+  <si>
+    <t>20.  Allow bulk deleting of rows in a grid.</t>
+  </si>
+  <si>
+    <t>21.  Create functionality to allow the object and collection to dump its state. See Serialisable</t>
+  </si>
+  <si>
+    <t>29.  Collapsible Panel</t>
+  </si>
+  <si>
+    <t>8.      Generate Database Structure and manage versions of application with different databases. (dep 1)</t>
+  </si>
+  <si>
+    <t>5.      Relationships define philosophy and implement</t>
+  </si>
+  <si>
+    <t>4.      Lookups Define philosophy and rework</t>
+  </si>
+  <si>
+    <t>e.       Save the Business Model to XML instead of a database</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +923,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1202,6 +971,30 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1211,28 +1004,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
@@ -1533,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1548,34 +1332,34 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="17"/>
+    <row r="2" spans="1:6" ht="15.75">
+      <c r="A2" s="25"/>
       <c r="B2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="25" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A3" s="19"/>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A3" s="27"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" thickBot="1">
+    <row r="4" spans="1:6" ht="16.5" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1586,24 +1370,27 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="32.25" thickBot="1">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:6" ht="30.75" thickBot="1">
+      <c r="A5" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18">
+        <v>4</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32.25" thickBot="1">
+      <c r="A6" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="1:5" ht="32.25" thickBot="1">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2">
         <v>8</v>
@@ -1612,28 +1399,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="63.75" thickBot="1">
+    <row r="7" spans="1:6" ht="63.75" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="32.25" thickBot="1">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
+      <c r="E7" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30.75" thickBot="1">
+      <c r="A8" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -1642,24 +1429,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
+    <row r="9" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A9" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" thickBot="1">
+      <c r="E9" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -1670,13 +1457,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.5" thickBot="1">
+    <row r="11" spans="1:6" ht="16.5" thickBot="1">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -1685,119 +1472,122 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A12" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
         <v>4</v>
       </c>
-      <c r="E12" s="20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A13" s="3" t="s">
-        <v>15</v>
+      <c r="E12" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" thickBot="1">
+      <c r="A13" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2">
         <v>12</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A14" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="18">
         <v>2</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" thickBot="1">
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" thickBot="1">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" ht="16.5" thickBot="1">
+      <c r="E15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2">
         <v>2</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16.5" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="22">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32.25" thickBot="1">
       <c r="A18" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2">
         <v>4</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16.5" thickBot="1">
       <c r="A19" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="22">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="32.25" thickBot="1">
-      <c r="A20" s="3" t="s">
-        <v>22</v>
+    <row r="20" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A20" s="30" t="s">
+        <v>53</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="2"/>
@@ -1805,85 +1595,85 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A21" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="21">
+      <c r="A21" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="18">
         <v>4</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75">
       <c r="A22" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17">
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75">
       <c r="A23" s="7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
     </row>
     <row r="25" spans="1:5" ht="16.5" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A26" s="3" t="s">
-        <v>27</v>
+      <c r="A26" s="23" t="s">
+        <v>48</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" ht="16.5" thickBot="1">
       <c r="A27" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="16.5" thickBot="1">
       <c r="A28" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="2"/>
@@ -1896,7 +1686,7 @@
     </row>
     <row r="29" spans="1:5" ht="16.5" thickBot="1">
       <c r="A29" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="2"/>
@@ -1905,28 +1695,28 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32.25" thickBot="1">
-      <c r="A30" s="3" t="s">
-        <v>32</v>
+    <row r="30" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A30" s="23" t="s">
+        <v>49</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" s="2">
         <v>1</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="17">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="16.5" thickBot="1">
       <c r="A31" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D31" s="2">
         <v>3</v>
@@ -1937,11 +1727,11 @@
     </row>
     <row r="32" spans="1:5" ht="16.5" thickBot="1">
       <c r="A32" s="10" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" s="11">
         <v>1</v>
@@ -1952,7 +1742,7 @@
     </row>
     <row r="33" spans="1:5" ht="16.5" thickBot="1">
       <c r="A33" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="2"/>
@@ -1965,74 +1755,74 @@
     </row>
     <row r="34" spans="1:5" ht="16.5" thickBot="1">
       <c r="A34" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="20">
+      <c r="E34" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A35" s="3" t="s">
-        <v>37</v>
+      <c r="A35" s="23" t="s">
+        <v>50</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35" s="2">
         <v>1</v>
       </c>
-      <c r="E35" s="20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="32.25" thickBot="1">
-      <c r="A36" s="3" t="s">
-        <v>38</v>
+      <c r="E35" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A36" s="23" t="s">
+        <v>51</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D36" s="2">
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="48" thickBot="1">
       <c r="A37" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2">
         <v>3</v>
       </c>
-      <c r="E37" s="20">
+      <c r="E37" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" thickBot="1">
       <c r="A38" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2">
         <v>4</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16.5" thickBot="1">
       <c r="A39" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="2"/>
@@ -2040,16 +1830,16 @@
         <v>2</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16.5" thickBot="1">
       <c r="A40" s="10" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B40" s="16"/>
       <c r="C40" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D40" s="11">
         <v>2</v>
@@ -2060,18 +1850,18 @@
     </row>
     <row r="41" spans="1:5" ht="16.5" thickBot="1">
       <c r="A41" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" ht="16.5" thickBot="1">
       <c r="A42" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="2"/>
@@ -2079,16 +1869,16 @@
         <v>12</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16.5" thickBot="1">
       <c r="A43" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D43" s="2">
         <v>1</v>
@@ -2098,8 +1888,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A44" s="3" t="s">
-        <v>49</v>
+      <c r="A44" s="23" t="s">
+        <v>52</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="2"/>
@@ -2112,7 +1902,7 @@
     </row>
     <row r="45" spans="1:5" ht="16.5" thickBot="1">
       <c r="A45" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="2"/>
@@ -2124,16 +1914,21 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A46" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24">
+      <c r="A46" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21">
         <v>1</v>
       </c>
-      <c r="E46" s="24">
+      <c r="E46" s="21">
         <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75">
+      <c r="A47" s="32" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added items to this todo
</commit_message>
<xml_diff>
--- a/docs/PriorityList.xlsx
+++ b/docs/PriorityList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="108">
   <si>
     <t>Started W/out peter</t>
   </si>
@@ -891,6 +891,15 @@
   </si>
   <si>
     <t>InsertOrdering - When have Many to many</t>
+  </si>
+  <si>
+    <t>Nice to have from Use Case Manager</t>
+  </si>
+  <si>
+    <t>DataStoreInMemory saves to .xml in addition to .dat</t>
+  </si>
+  <si>
+    <t>Percentage defined width property on UI Grids so that columns will fit to screen (like table width in html)</t>
   </si>
 </sst>
 </file>
@@ -1163,18 +1172,18 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
@@ -1473,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1492,14 +1501,14 @@
       <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="15.75">
-      <c r="A2" s="31"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="34" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1507,10 +1516,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1">
-      <c r="A3" s="33"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1776,9 +1785,9 @@
         <v>16</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34">
         <v>7</v>
       </c>
     </row>
@@ -1787,27 +1796,27 @@
         <v>17</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
     </row>
     <row r="25" spans="1:5" ht="16.5" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:5" ht="16.5" thickBot="1">
       <c r="A26" s="23" t="s">
@@ -2172,52 +2181,52 @@
       </c>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="31" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="34" t="s">
+      <c r="A59" s="31" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="34" t="s">
+      <c r="A60" s="31" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="34" t="s">
+      <c r="A61" s="31" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="34" t="s">
+      <c r="A62" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="34" t="s">
+      <c r="A63" s="31" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="34" t="s">
+      <c r="A64" s="31" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="31" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="34" t="s">
+      <c r="A66" s="31" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="34" t="s">
+      <c r="A67" s="31" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2227,27 +2236,27 @@
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="31" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="34" t="s">
+      <c r="A70" s="31" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="35" t="s">
+      <c r="A71" s="32" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="36" t="s">
+      <c r="A72" s="33" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="35" t="s">
+      <c r="A73" s="32" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2319,6 +2328,21 @@
     <row r="87" spans="1:1">
       <c r="A87" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>